<commit_message>
Frontend: Changed home page design, Made pages responsive
</commit_message>
<xml_diff>
--- a/templates/expense_template.xlsx
+++ b/templates/expense_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aakas\OneDrive\Documents\UWA\2nd_intermediate_deliverable\Budget-Manager\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaewon/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629A19AA-2076-4843-BFDD-F339E9622525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6942FA6F-855A-E243-AC13-4836BF71AFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32265" yWindow="3465" windowWidth="21600" windowHeight="11385" xr2:uid="{7CE38616-C7AF-374A-AA4F-A9EBB69AB0C1}"/>
+    <workbookView xWindow="-24420" yWindow="-1220" windowWidth="24340" windowHeight="20760" xr2:uid="{7CE38616-C7AF-374A-AA4F-A9EBB69AB0C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,6 +57,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -86,8 +89,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,15 +430,17 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="11" style="1"/>
+    <col min="4" max="4" width="11" style="2"/>
     <col min="5" max="5" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -451,6 +458,14 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{0D8A7E96-3694-274C-9899-AB74459BE153}">
+      <formula1>"Rent,Travel,Entertainment,Utilities,Groceries,Insurance,Debt Repayments,Loan,Medical"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{6B84B75F-2695-D542-9980-F24C13C9B16E}">
+      <formula1>"Mobile Wallet,Credit Card,Cash,Bank Transfer,Debit Card,Other"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>